<commit_message>
updated saucedemo practice module
</commit_message>
<xml_diff>
--- a/saucedemo_practice/excelfile/login_input.xlsx
+++ b/saucedemo_practice/excelfile/login_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pytest_learning\saucedemo_practice\excelfile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75AEABFF-E15E-4AAC-AB3B-D40FB414B974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{315BF691-9622-497C-BE0A-204B76338429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2904" yWindow="1512" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,10 +61,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF4A4A4A"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -87,9 +95,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -373,52 +382,53 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>